<commit_message>
Esclarecendo melhor como funciona aimportação de leads
</commit_message>
<xml_diff>
--- a/res/modelo_leads_b2b.xlsx
+++ b/res/modelo_leads_b2b.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace-VSCode\job\treinamento-ploomes - Copia\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDFCE4A-40B6-440B-9BD8-2B5DBEE3DD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7AB9C2-2A5E-4E2E-BFF9-27208A137398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C2432BDF-6794-4D67-9C2F-0804784596A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C2432BDF-6794-4D67-9C2F-0804784596A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>(Contato) CNPJ</t>
   </si>
@@ -69,13 +69,19 @@
   </si>
   <si>
     <t>(Cliente) Advogado Nome</t>
+  </si>
+  <si>
+    <t>(Negócio) Estágio</t>
+  </si>
+  <si>
+    <t>Novo Lead</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,8 +89,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,8 +111,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -106,13 +126,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,8 +182,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AAD40563-063E-4FF7-99EA-BCF86DB9D62C}" name="Tabela1" displayName="Tabela1" ref="A1:F2" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:F2" xr:uid="{AAD40563-063E-4FF7-99EA-BCF86DB9D62C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AAD40563-063E-4FF7-99EA-BCF86DB9D62C}" name="Tabela1" displayName="Tabela1" ref="B1:G2" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B1:G2" xr:uid="{AAD40563-063E-4FF7-99EA-BCF86DB9D62C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{AB94AA61-8DE8-499C-BAD6-746DB7C28578}" name="(Negócio) Título"/>
     <tableColumn id="2" xr3:uid="{5D22AD44-81C4-4101-B9F9-83777B2F3E26}" name="(Negócio) Responsável"/>
@@ -471,55 +513,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A88D1C-09E8-4D83-9503-19D753C7E143}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>123456789</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>